<commit_message>
example input data frames
</commit_message>
<xml_diff>
--- a/data-raw/forestindicators_input.xlsx
+++ b/data-raw/forestindicators_input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nuria.aquilue\Generalitat de Catalunya\NAquilué - General\COLLABORATIONS\EMF\forestindicators\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gencat.sharepoint.com/sites/CTFC_NAquilu/Documents compartits/General/COLLABORATIONS/EMF/forestindicators/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C03D9AB-CFF9-420A-932D-3383812415BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{2C03D9AB-CFF9-420A-932D-3383812415BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EEAE082-A1DB-48F8-B706-BC24553D94E2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,19 @@
     <sheet name="indicators" sheetId="1" r:id="rId1"/>
     <sheet name="variables" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -26,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
   <si>
     <t>stand_static_variables</t>
   </si>
@@ -127,15 +138,9 @@
     <t>slope</t>
   </si>
   <si>
-    <t>mean_annual_precipitation, canopy_cover</t>
-  </si>
-  <si>
     <t>timber_harvest_01</t>
   </si>
   <si>
-    <t>state, species, dbh, h, n</t>
-  </si>
-  <si>
     <t>stand</t>
   </si>
   <si>
@@ -190,9 +195,6 @@
     <t>degree of beautiness of plant; value 0 (low) - 1 (high)</t>
   </si>
   <si>
-    <t>state, species, dbh, n</t>
-  </si>
-  <si>
     <t>variable</t>
   </si>
   <si>
@@ -206,6 +208,30 @@
   </si>
   <si>
     <t>density</t>
+  </si>
+  <si>
+    <t>º</t>
+  </si>
+  <si>
+    <t>slope in degrees</t>
+  </si>
+  <si>
+    <t>mean_precipitation</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean precipitation for the time period </t>
+  </si>
+  <si>
+    <t>mean_precipitation, canopy_cover</t>
+  </si>
+  <si>
+    <t>state, dbh, n</t>
+  </si>
+  <si>
+    <t>state, dbh, h, n</t>
   </si>
 </sst>
 </file>
@@ -449,7 +475,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -541,7 +567,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -553,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
         <v>16</v>
@@ -561,16 +587,16 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" t="s">
-        <v>50</v>
-      </c>
       <c r="H4" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -581,10 +607,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,13 +621,13 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>18</v>
@@ -612,172 +638,206 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
+        <v>42</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
         <v>45</v>
       </c>
-      <c r="E11" t="s">
-        <v>53</v>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data new density_dead_wood indicator
</commit_message>
<xml_diff>
--- a/data-raw/forestindicators_input.xlsx
+++ b/data-raw/forestindicators_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gencat.sharepoint.com/sites/CTFC_NAquilu/Documents compartits/General/COLLABORATIONS/EMF/forestindicators/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_1261C2370B682EC8ABFD32753885C117BD985D05" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F9CE67B-78B8-49C1-A885-E944C86F4606}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_1261C2370B682EC8ABFD32753885C117BD985D05" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C65A9D5-8629-4CEC-A48C-3B97EDE1ED87}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
   <si>
     <t>indicator</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>degree of beautiness of plant; value 0 (low) - 1 (high)</t>
+  </si>
+  <si>
+    <t>density_dead_wood</t>
+  </si>
+  <si>
+    <t>Density of large dead wood. By default, large dead tree is as DBH &gt;= 17.5 cm</t>
   </si>
 </sst>
 </file>
@@ -465,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,6 +577,20 @@
       </c>
       <c r="F4" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -830,6 +850,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="10b2415f-6b16-408d-a5df-bf55a3837e9c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095DDF5E8B92F09488F6994CC76A3261F" ma:contentTypeVersion="14" ma:contentTypeDescription="Crea un document nou" ma:contentTypeScope="" ma:versionID="77fb5a445c241a114a6db4ced5f4c9a2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="10b2415f-6b16-408d-a5df-bf55a3837e9c" xmlns:ns3="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a9fed371820f3b6ac84a8d3142ba9e2" ns2:_="" ns3:_="">
     <xsd:import namespace="10b2415f-6b16-408d-a5df-bf55a3837e9c"/>
@@ -1042,17 +1073,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="10b2415f-6b16-408d-a5df-bf55a3837e9c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBDEF4A3-9AF9-4E88-BFDA-A0306FB881A6}">
   <ds:schemaRefs>
@@ -1062,6 +1082,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07A91501-B07B-4C88-A941-795638A5577F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8"/>
+    <ds:schemaRef ds:uri="10b2415f-6b16-408d-a5df-bf55a3837e9c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB7D4ED6-746B-48CE-AEFA-75DD54485591}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1078,15 +1109,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07A91501-B07B-4C88-A941-795638A5577F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8"/>
-    <ds:schemaRef ds:uri="10b2415f-6b16-408d-a5df-bf55a3837e9c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
dominant tree height and diameter
</commit_message>
<xml_diff>
--- a/data-raw/forestindicators_input.xlsx
+++ b/data-raw/forestindicators_input.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="98">
   <si>
     <t xml:space="preserve">indicator</t>
   </si>
@@ -69,12 +69,30 @@
     <t xml:space="preserve">Miquel De Cáceres</t>
   </si>
   <si>
+    <t xml:space="preserve">dominant_tree_height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">state, dbh, h, n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dominant tree height, i.e the average height of the 100 tallest trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dominant_tree_diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dominant tree diameter, i.e the average diameter of the 100 tallest trees</t>
+  </si>
+  <si>
     <t xml:space="preserve">timber_harvest</t>
   </si>
   <si>
-    <t xml:space="preserve">state, dbh, h, n</t>
-  </si>
-  <si>
     <t xml:space="preserve">Volume over bark of harvested wood</t>
   </si>
   <si>
@@ -144,6 +162,12 @@
     <t xml:space="preserve">Status of trees included in estimation of basal area</t>
   </si>
   <si>
+    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of dominant tree height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of dominant tree diameter</t>
+  </si>
+  <si>
     <t xml:space="preserve">province</t>
   </si>
   <si>
@@ -246,9 +270,6 @@
     <t xml:space="preserve">dominant_dbh</t>
   </si>
   <si>
-    <t xml:space="preserve">cm</t>
-  </si>
-  <si>
     <t xml:space="preserve">dbh of the 100 dominant trees</t>
   </si>
   <si>
@@ -280,9 +301,6 @@
   </si>
   <si>
     <t xml:space="preserve">h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
   </si>
   <si>
     <t xml:space="preserve">height</t>
@@ -587,15 +605,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:XFD9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.45"/>
@@ -659,75 +677,129 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="I3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="XFB3" s="1"/>
+      <c r="XFC3" s="1"/>
+      <c r="XFD3" s="1"/>
+    </row>
+    <row r="4" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="XFB4" s="0"/>
+      <c r="XFC4" s="0"/>
+      <c r="XFD4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="3" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="3" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="I7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="XFB7" s="3"/>
+      <c r="XFC7" s="3"/>
+      <c r="XFD7" s="3"/>
+    </row>
+    <row r="8" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="XFB9" s="1"/>
+      <c r="XFC9" s="1"/>
+      <c r="XFD9" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -745,10 +817,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -764,13 +836,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -778,13 +850,13 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,115 +864,143 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
+      <c r="A5" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -933,223 +1033,223 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
quadratic mean tree diameter
</commit_message>
<xml_diff>
--- a/data-raw/forestindicators_input.xlsx
+++ b/data-raw/forestindicators_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="indicators" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="104">
   <si>
     <t xml:space="preserve">indicator</t>
   </si>
@@ -78,6 +78,9 @@
     <t xml:space="preserve">m</t>
   </si>
   <si>
+    <t xml:space="preserve">The average height of the 100 tallest trees, excluding dead trees and trees of diameter smaller than threshold</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dominant tree height, i.e the average height of the 100 tallest trees</t>
   </si>
   <si>
@@ -87,7 +90,19 @@
     <t xml:space="preserve">cm</t>
   </si>
   <si>
-    <t xml:space="preserve">Dominant tree diameter, i.e the average diameter of the 100 tallest trees</t>
+    <t xml:space="preserve">The average diameter of the 100 largest trees, excluding dead trees and trees of diameter smaller than threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dominant tree diameter, i.e the average diameter of the 100 largest trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quadratic_mean_tree_diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invert the calculation of tree section after dividing basal area by tree density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quadratic mean tree diameter, i.e. the diameter value corresponding to the current basal area and density</t>
   </si>
   <si>
     <t xml:space="preserve">timber_harvest</t>
@@ -166,6 +181,9 @@
   </si>
   <si>
     <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of dominant tree diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of quadratic mean tree diameter</t>
   </si>
   <si>
     <t xml:space="preserve">province</t>
@@ -605,15 +623,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD9"/>
+  <dimension ref="A1:XFD10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.45"/>
@@ -690,9 +708,11 @@
       <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="H3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>14</v>
@@ -703,7 +723,7 @@
     </row>
     <row r="4" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -712,94 +732,122 @@
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="H4" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="XFB4" s="0"/>
-      <c r="XFC4" s="0"/>
-      <c r="XFD4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="XFB4" s="1"/>
+      <c r="XFC4" s="1"/>
+      <c r="XFD4" s="1"/>
+    </row>
+    <row r="5" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="XFB5" s="1"/>
+      <c r="XFC5" s="1"/>
+      <c r="XFD5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="XFB7" s="3"/>
-      <c r="XFC7" s="3"/>
-      <c r="XFD7" s="3"/>
-    </row>
-    <row r="8" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="H8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="XFB8" s="3"/>
+      <c r="XFC8" s="3"/>
+      <c r="XFD8" s="3"/>
     </row>
     <row r="9" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="G9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="XFB9" s="1"/>
-      <c r="XFC9" s="1"/>
-      <c r="XFD9" s="1"/>
+      <c r="XFB10" s="1"/>
+      <c r="XFC10" s="1"/>
+      <c r="XFD10" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -817,9 +865,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -836,13 +884,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,13 +898,13 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -864,13 +912,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,129 +926,143 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
+      <c r="A6" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1022,7 +1084,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1033,223 +1095,223 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
carbon stock and timber harvest revisited
</commit_message>
<xml_diff>
--- a/data-raw/forestindicators_input.xlsx
+++ b/data-raw/forestindicators_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="indicators" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="137">
   <si>
     <t xml:space="preserve">indicator</t>
   </si>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">implementation_responsible</t>
   </si>
   <si>
-    <t xml:space="preserve">basal_area</t>
+    <t xml:space="preserve">live_basal_area</t>
   </si>
   <si>
     <t xml:space="preserve">state, dbh, n</t>
@@ -60,16 +60,31 @@
     <t xml:space="preserve">m2/ha</t>
   </si>
   <si>
-    <t xml:space="preserve">The sum of tree sections weighted by tree density of trees larger than a pre-specified minimum parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basal area of the stand (focusing of living trees by default)</t>
+    <t xml:space="preserve">The sum of tree sections weighted by tree density of living trees larger than a pre-specified minimum parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basal area of the stand, focusing of living trees</t>
   </si>
   <si>
     <t xml:space="preserve">Miquel De Cáceres</t>
   </si>
   <si>
-    <t xml:space="preserve">tree_density</t>
+    <t xml:space="preserve">dead_basal_area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sum of tree sections weighted by tree density of dead trees larger than a pre-specified minimum parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cut_basal_area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sum of tree sections weighted by tree density of cut trees larger than a pre-specified minimum parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basal area of the stand, focusing of cut trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">live_tree_density</t>
   </si>
   <si>
     <t xml:space="preserve">ind/ha</t>
@@ -81,6 +96,24 @@
     <t xml:space="preserve">Density of living trees per hectare</t>
   </si>
   <si>
+    <t xml:space="preserve">dead_tree_density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of dead trees larger than minimum diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Density of dead trees per hectare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cut_tree_density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of cut trees larger than minimum diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Density of cut trees per hectare</t>
+  </si>
+  <si>
     <t xml:space="preserve">dominant_tree_height</t>
   </si>
   <si>
@@ -141,21 +174,60 @@
     <t xml:space="preserve">timber_harvest</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">state, dbh, h, n, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">plant_entity</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">m3/ha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allometric relationships published with the Spanish National Forest Inventory</t>
+  </si>
+  <si>
     <t xml:space="preserve">Volume over bark of harvested wood</t>
   </si>
   <si>
+    <t xml:space="preserve">Núria Aquilué / Miquel De Cáceres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carbon_stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mg/ha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allometric relationships published by INIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total biomass of living trees, including aboveground and belowground components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">density_dead_wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Density of large dead wood. By default, large dead tree is as DBH &gt;= 17.5 cm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Núria Aquilué</t>
   </si>
   <si>
-    <t xml:space="preserve">carbon_stock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">density_dead_wood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Density of large dead wood. By default, large dead tree is as DBH &gt;= 17.5 cm</t>
-  </si>
-  <si>
     <t xml:space="preserve">soil_erosion_rusle</t>
   </si>
   <si>
@@ -198,19 +270,22 @@
     <t xml:space="preserve">7.5</t>
   </si>
   <si>
-    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of basal area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tree_state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“live”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status of trees included in estimation of basal area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of tree density</t>
+    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of basal area of live trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of basal area of dead trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of basal area of cut trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of density of live trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of density of dead trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of density of cut trees</t>
   </si>
   <si>
     <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of dominant tree height</t>
@@ -228,12 +303,6 @@
     <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of hart-becking index</t>
   </si>
   <si>
-    <t xml:space="preserve">province</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spanish province (numeric code)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of harvest volume</t>
   </si>
   <si>
@@ -255,6 +324,15 @@
     <t xml:space="preserve">Tree species not included in the calculation of harvested volume</t>
   </si>
   <si>
+    <t xml:space="preserve">fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“total”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A string, either "total" (for total biomass), "stem" (for stem biomass), "branches" (for branch biomass), "aboveground" (for aboveground biomass) or "belowground" (for belowground biomass).</t>
+  </si>
+  <si>
     <t xml:space="preserve">Plant species included in the calculation of carbon stock</t>
   </si>
   <si>
@@ -342,10 +420,10 @@
     <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t xml:space="preserve">state of the cohort, tree, … can be 'live', 'cut', or 'death'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">species</t>
+    <t xml:space="preserve">state of the cohort, tree, … can be 'live', 'cut', or 'dead'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plant_entity</t>
   </si>
   <si>
     <t xml:space="preserve">name or code? of the tree, shrub, … species</t>
@@ -382,7 +460,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +490,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -662,10 +746,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD13"/>
+  <dimension ref="A1:XFD17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -674,7 +758,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="61.56"/>
@@ -745,13 +829,13 @@
         <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>14</v>
@@ -759,33 +843,30 @@
     </row>
     <row r="4" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="XFB4" s="1"/>
-      <c r="XFC4" s="1"/>
-      <c r="XFD4" s="1"/>
     </row>
     <row r="5" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -794,13 +875,13 @@
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>14</v>
@@ -811,22 +892,22 @@
     </row>
     <row r="6" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>14</v>
@@ -837,7 +918,7 @@
     </row>
     <row r="7" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -846,13 +927,13 @@
         <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>14</v>
@@ -863,22 +944,22 @@
     </row>
     <row r="8" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
+      <c r="E8" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>14</v>
@@ -887,81 +968,212 @@
       <c r="XFC8" s="1"/>
       <c r="XFD8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    <row r="9" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="XFB9" s="1"/>
+      <c r="XFC9" s="1"/>
+      <c r="XFD9" s="1"/>
+    </row>
+    <row r="10" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="H10" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="I10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="XFB10" s="1"/>
+      <c r="XFC10" s="1"/>
+      <c r="XFD10" s="1"/>
+    </row>
+    <row r="11" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="XFB11" s="3"/>
-      <c r="XFC11" s="3"/>
-      <c r="XFD11" s="3"/>
-    </row>
-    <row r="12" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="XFB11" s="1"/>
+      <c r="XFC11" s="1"/>
+      <c r="XFD11" s="1"/>
+    </row>
+    <row r="12" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="XFB12" s="1"/>
+      <c r="XFC12" s="1"/>
+      <c r="XFD12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="E13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="F13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="G13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="H13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="XFB13" s="3"/>
+      <c r="XFC13" s="3"/>
+      <c r="XFD13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="XFB14" s="3"/>
+      <c r="XFC14" s="3"/>
+      <c r="XFD14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="XFB16" s="1"/>
+      <c r="XFC16" s="1"/>
+      <c r="XFD16" s="1"/>
+    </row>
+    <row r="17" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="XFB13" s="1"/>
-      <c r="XFC13" s="1"/>
-      <c r="XFD13" s="1"/>
+      <c r="XFB17" s="1"/>
+      <c r="XFC17" s="1"/>
+      <c r="XFD17" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -979,10 +1191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -998,13 +1210,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1012,213 +1224,261 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>38</v>
+      <c r="A10" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>38</v>
+      <c r="A11" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>38</v>
+      <c r="A12" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>81</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1240,7 +1500,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1251,223 +1511,223 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new indicator: live tree volume stock
</commit_message>
<xml_diff>
--- a/data-raw/forestindicators_input.xlsx
+++ b/data-raw/forestindicators_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="indicators" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="145">
   <si>
     <t xml:space="preserve">indicator</t>
   </si>
@@ -189,6 +189,12 @@
     <t xml:space="preserve">Núria Aquilué / Miquel De Cáceres</t>
   </si>
   <si>
+    <t xml:space="preserve">live_tree_volume_stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume over bark of living trees</t>
+  </si>
+  <si>
     <t xml:space="preserve">live_tree_carbon_stock</t>
   </si>
   <si>
@@ -300,7 +306,7 @@
     <t xml:space="preserve">max_tree_dbh</t>
   </si>
   <si>
-    <t xml:space="preserve">Maximum  tree diameter to be included in the estimation of density of harvest volume</t>
+    <t xml:space="preserve">Maximum  tree diameter to be included in the estimation of harvest volume</t>
   </si>
   <si>
     <t xml:space="preserve">targeted_species</t>
@@ -313,6 +319,18 @@
   </si>
   <si>
     <t xml:space="preserve">Tree species not included in the calculation of harvested volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum  tree diameter to be included in the estimation of volume stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum  tree diameter to be included in the estimation of volume stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant species included in the calculation of volume stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant species not included in the calculation of volume stock</t>
   </si>
   <si>
     <t xml:space="preserve">Plant species included in the calculation of carbon stock</t>
@@ -728,10 +746,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD18"/>
+  <dimension ref="A1:XFD19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="1" sqref="A17:A20 A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1054,7 +1072,7 @@
       <c r="XFC12" s="1"/>
       <c r="XFD12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1077,7 +1095,7 @@
       <c r="XFC13" s="3"/>
       <c r="XFD13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -1085,36 +1103,36 @@
         <v>50</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>54</v>
+      <c r="I14" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="XFB14" s="3"/>
       <c r="XFC14" s="3"/>
       <c r="XFD14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>54</v>
@@ -1125,60 +1143,83 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>31</v>
+      <c r="G16" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>63</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="XFB16" s="3"/>
+      <c r="XFC16" s="3"/>
+      <c r="XFD16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="E17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="I17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="XFB17" s="1"/>
-      <c r="XFC17" s="1"/>
-      <c r="XFD17" s="1"/>
     </row>
     <row r="18" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>10</v>
+      <c r="I18" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="XFB18" s="1"/>
       <c r="XFC18" s="1"/>
       <c r="XFD18" s="1"/>
+    </row>
+    <row r="19" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="XFB19" s="1"/>
+      <c r="XFC19" s="1"/>
+      <c r="XFD19" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1196,10 +1237,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1215,13 +1256,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,13 +1270,13 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1243,13 +1284,13 @@
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1257,13 +1298,13 @@
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,13 +1312,13 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1285,13 +1326,13 @@
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1299,13 +1340,13 @@
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,13 +1354,13 @@
         <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,13 +1368,13 @@
         <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,13 +1382,13 @@
         <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1355,13 +1396,13 @@
         <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1369,13 +1410,13 @@
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1383,13 +1424,13 @@
         <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1397,10 +1438,10 @@
         <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,10 +1449,10 @@
         <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1419,10 +1460,10 @@
         <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,10 +1471,13 @@
         <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,57 +1485,101 @@
         <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1513,7 +1601,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="1" sqref="A17:A20 E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1524,223 +1612,223 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check input units when present
</commit_message>
<xml_diff>
--- a/data-raw/forestindicators_input.xlsx
+++ b/data-raw/forestindicators_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="indicators" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="144">
   <si>
     <t xml:space="preserve">indicator</t>
   </si>
@@ -225,7 +225,7 @@
     <t xml:space="preserve">soil_erosion_rusle</t>
   </si>
   <si>
-    <t xml:space="preserve">slope</t>
+    <t xml:space="preserve">slope_degree</t>
   </si>
   <si>
     <t xml:space="preserve">mean_precipitation, canopy_cover</t>
@@ -375,19 +375,25 @@
     <t xml:space="preserve">area of the stand</t>
   </si>
   <si>
-    <t xml:space="preserve">º</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slope in degrees</t>
+    <t xml:space="preserve">degree_north</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slope in degrees from north</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slope_percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slope in percent</t>
   </si>
   <si>
     <t xml:space="preserve">mean_temperature</t>
   </si>
   <si>
-    <t xml:space="preserve">º C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean temperature for the time period </t>
+    <t xml:space="preserve">celsius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean temperature for the time period in degree Celsius</t>
   </si>
   <si>
     <t xml:space="preserve">mean_precipitation</t>
@@ -420,9 +426,6 @@
     <t xml:space="preserve">character</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
     <t xml:space="preserve">state of the cohort, tree, … can be 'live', 'cut', or 'dead'</t>
   </si>
   <si>
@@ -445,9 +448,6 @@
   </si>
   <si>
     <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ind./ha</t>
   </si>
   <si>
     <t xml:space="preserve">density</t>
@@ -537,7 +537,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -552,6 +552,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -745,8 +749,8 @@
   </sheetPr>
   <dimension ref="A1:XFD19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1595,15 +1599,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="44.11"/>
   </cols>
   <sheetData>
@@ -1641,7 +1646,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -1651,7 +1656,7 @@
       <c r="C3" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>117</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1669,15 +1674,15 @@
         <v>114</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>113</v>
@@ -1686,15 +1691,15 @@
         <v>114</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>113</v>
@@ -1703,7 +1708,7 @@
         <v>114</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>126</v>
@@ -1720,7 +1725,7 @@
         <v>114</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>128</v>
@@ -1731,100 +1736,111 @@
         <v>129</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>

<commit_message>
timber harvest carbon rate
</commit_message>
<xml_diff>
--- a/data-raw/forestindicators_input.xlsx
+++ b/data-raw/forestindicators_input.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="152">
   <si>
     <t xml:space="preserve">indicator</t>
   </si>
@@ -222,6 +222,12 @@
     <t xml:space="preserve">Annual rate of change in biomass of living tree in CO2 equivalent, including aboveground and belowground components. Positive values mean sequestration.</t>
   </si>
   <si>
+    <t xml:space="preserve">timber_harvest_carbon_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual rate of CO2 equivalents due to timber harvest, including stem biomass component only. Positive values mean sequestration.</t>
+  </si>
+  <si>
     <t xml:space="preserve">density_dead_wood</t>
   </si>
   <si>
@@ -352,6 +358,30 @@
   </si>
   <si>
     <t xml:space="preserve">Plant species not included in the calculation of live tree carbon change rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant species included in the calculation of timber harvest carbon rate</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Plant species not included in the calculation of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">timber harvest carbon rate</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">17.5</t>
@@ -475,7 +505,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,6 +535,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -759,10 +795,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD20"/>
+  <dimension ref="A1:XFD21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1202,57 +1238,77 @@
         <v>66</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="XFB18" s="3"/>
+      <c r="XFC18" s="3"/>
+      <c r="XFD18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="19" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="E19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="I19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="XFB19" s="1"/>
-      <c r="XFC19" s="1"/>
-      <c r="XFD19" s="1"/>
     </row>
     <row r="20" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>10</v>
+      <c r="I20" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="XFB20" s="1"/>
       <c r="XFC20" s="1"/>
       <c r="XFD20" s="1"/>
+    </row>
+    <row r="21" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="XFB21" s="1"/>
+      <c r="XFC21" s="1"/>
+      <c r="XFD21" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1270,10 +1326,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1048576"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1289,13 +1345,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1303,13 +1359,13 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1317,13 +1373,13 @@
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1331,13 +1387,13 @@
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1345,13 +1401,13 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1359,13 +1415,13 @@
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1373,13 +1429,13 @@
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1387,13 +1443,13 @@
         <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,13 +1457,13 @@
         <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1415,13 +1471,13 @@
         <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,13 +1485,13 @@
         <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,13 +1499,13 @@
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1457,13 +1513,13 @@
         <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1471,10 +1527,10 @@
         <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1482,10 +1538,10 @@
         <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,10 +1549,10 @@
         <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,13 +1560,13 @@
         <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,10 +1574,10 @@
         <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1529,10 +1585,10 @@
         <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,10 +1596,10 @@
         <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,10 +1607,10 @@
         <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,10 +1618,10 @@
         <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,10 +1629,10 @@
         <v>61</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,10 +1640,10 @@
         <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1595,10 +1651,10 @@
         <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1606,10 +1662,10 @@
         <v>63</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,27 +1673,48 @@
         <v>66</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1669,231 +1746,231 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>